<commit_message>
Google pivot test summary.
</commit_message>
<xml_diff>
--- a/pivot/time.xlsx
+++ b/pivot/time.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B77B22BE-90D5-4C43-A47C-8ACE36381865}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Slashdot" sheetId="1" r:id="rId1"/>
@@ -13,7 +12,7 @@
     <sheet name="Google" sheetId="4" r:id="rId3"/>
     <sheet name="Sheet1" sheetId="2" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -84,7 +83,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -134,9 +133,9 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="da-DK"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -173,6 +172,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -281,7 +281,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-C401-40F5-B060-A3F60EFA96E4}"/>
             </c:ext>
@@ -359,7 +359,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-C401-40F5-B060-A3F60EFA96E4}"/>
             </c:ext>
@@ -437,7 +437,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-C401-40F5-B060-A3F60EFA96E4}"/>
             </c:ext>
@@ -515,7 +515,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000003-C401-40F5-B060-A3F60EFA96E4}"/>
             </c:ext>
@@ -593,7 +593,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000004-C401-40F5-B060-A3F60EFA96E4}"/>
             </c:ext>
@@ -671,7 +671,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-7C12-45DC-ACD4-01A03356F631}"/>
             </c:ext>
@@ -687,11 +687,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="2053589135"/>
-        <c:axId val="2051979647"/>
+        <c:axId val="244130256"/>
+        <c:axId val="244130648"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2053589135"/>
+        <c:axId val="244130256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -734,7 +734,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2051979647"/>
+        <c:crossAx val="244130648"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -742,7 +742,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2051979647"/>
+        <c:axId val="244130648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -793,7 +793,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2053589135"/>
+        <c:crossAx val="244130256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -807,6 +807,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -838,14 +839,14 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:extLst>
+    <c:showDLblsOverMax val="0"/>
+    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
           <c16r3:dispNaAsBlank val="1"/>
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -881,9 +882,9 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="da-DK"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -920,6 +921,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1042,7 +1044,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-E173-44B3-BDEB-F21D546923FF}"/>
             </c:ext>
@@ -1135,7 +1137,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-E173-44B3-BDEB-F21D546923FF}"/>
             </c:ext>
@@ -1228,7 +1230,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-E173-44B3-BDEB-F21D546923FF}"/>
             </c:ext>
@@ -1321,7 +1323,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000003-E173-44B3-BDEB-F21D546923FF}"/>
             </c:ext>
@@ -1414,7 +1416,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000004-E173-44B3-BDEB-F21D546923FF}"/>
             </c:ext>
@@ -1507,7 +1509,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-683D-4A22-9D87-132F005A1AE9}"/>
             </c:ext>
@@ -1523,11 +1525,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2058885663"/>
-        <c:axId val="2046668255"/>
+        <c:axId val="244131432"/>
+        <c:axId val="244131824"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2058885663"/>
+        <c:axId val="244131432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1570,7 +1572,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2046668255"/>
+        <c:crossAx val="244131824"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1578,7 +1580,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2046668255"/>
+        <c:axId val="244131824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1629,7 +1631,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2058885663"/>
+        <c:crossAx val="244131432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1643,6 +1645,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1674,14 +1677,14 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:extLst>
+    <c:showDLblsOverMax val="0"/>
+    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
           <c16r3:dispNaAsBlank val="1"/>
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -1717,9 +1720,9 @@
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="da-DK"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1756,6 +1759,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1869,7 +1873,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-1BEC-4819-8FF4-A62DD3E188D4}"/>
             </c:ext>
@@ -1952,7 +1956,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-1BEC-4819-8FF4-A62DD3E188D4}"/>
             </c:ext>
@@ -2035,7 +2039,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-1BEC-4819-8FF4-A62DD3E188D4}"/>
             </c:ext>
@@ -2118,7 +2122,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000003-1BEC-4819-8FF4-A62DD3E188D4}"/>
             </c:ext>
@@ -2201,7 +2205,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000004-1BEC-4819-8FF4-A62DD3E188D4}"/>
             </c:ext>
@@ -2217,11 +2221,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="817294175"/>
-        <c:axId val="823995663"/>
+        <c:axId val="246000840"/>
+        <c:axId val="246001232"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="817294175"/>
+        <c:axId val="246000840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2264,7 +2268,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="823995663"/>
+        <c:crossAx val="246001232"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2272,7 +2276,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="823995663"/>
+        <c:axId val="246001232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2323,7 +2327,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="817294175"/>
+        <c:crossAx val="246000840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2337,6 +2341,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2404,9 +2409,9 @@
 </file>
 
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="da-DK"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2443,6 +2448,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2565,7 +2571,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-D0C5-4BF8-8DFF-DCD9611F9A16}"/>
             </c:ext>
@@ -2658,7 +2664,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-D0C5-4BF8-8DFF-DCD9611F9A16}"/>
             </c:ext>
@@ -2751,7 +2757,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-D0C5-4BF8-8DFF-DCD9611F9A16}"/>
             </c:ext>
@@ -2844,7 +2850,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000003-D0C5-4BF8-8DFF-DCD9611F9A16}"/>
             </c:ext>
@@ -2937,7 +2943,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000004-D0C5-4BF8-8DFF-DCD9611F9A16}"/>
             </c:ext>
@@ -3030,7 +3036,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-4F0C-47B3-8F61-B301D1226146}"/>
             </c:ext>
@@ -3046,11 +3052,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="922613247"/>
-        <c:axId val="816115151"/>
+        <c:axId val="246002016"/>
+        <c:axId val="246002408"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="922613247"/>
+        <c:axId val="246002016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3093,7 +3099,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="816115151"/>
+        <c:crossAx val="246002408"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3101,7 +3107,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="816115151"/>
+        <c:axId val="246002408"/>
         <c:scaling>
           <c:logBase val="2"/>
           <c:orientation val="minMax"/>
@@ -3154,7 +3160,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="922613247"/>
+        <c:crossAx val="246002016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3168,6 +3174,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3199,14 +3206,14 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:extLst>
+    <c:showDLblsOverMax val="0"/>
+    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
           <c16r3:dispNaAsBlank val="1"/>
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -3242,9 +3249,9 @@
 </file>
 
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="da-DK"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -3281,6 +3288,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3374,27 +3382,27 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>290463</c:v>
+                  <c:v>99137.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>268599</c:v>
+                  <c:v>81427</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>19405.5</c:v>
+                  <c:v>20272</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10493</c:v>
+                  <c:v>1751.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>10574</c:v>
+                  <c:v>1729.5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>10577</c:v>
+                  <c:v>1791.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-6DCB-4C1A-9A89-E3180E619432}"/>
             </c:ext>
@@ -3457,27 +3465,27 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>193442.5</c:v>
+                  <c:v>54961</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>188385.5</c:v>
+                  <c:v>45044.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>11636</c:v>
+                  <c:v>10361.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6072.5</c:v>
+                  <c:v>1047</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6156.5</c:v>
+                  <c:v>1023</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6277</c:v>
+                  <c:v>1097.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-6DCB-4C1A-9A89-E3180E619432}"/>
             </c:ext>
@@ -3540,27 +3548,27 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>148057</c:v>
+                  <c:v>36972.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>130012</c:v>
+                  <c:v>32644</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7101</c:v>
+                  <c:v>5550.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3469.5</c:v>
+                  <c:v>653.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3552</c:v>
+                  <c:v>632</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3635.5</c:v>
+                  <c:v>713.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-6DCB-4C1A-9A89-E3180E619432}"/>
             </c:ext>
@@ -3623,27 +3631,27 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>78329.5</c:v>
+                  <c:v>29082</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>71834.5</c:v>
+                  <c:v>27281</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4595.5</c:v>
+                  <c:v>3162.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2464.5</c:v>
+                  <c:v>463</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2441</c:v>
+                  <c:v>437</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2523.5</c:v>
+                  <c:v>553</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000003-6DCB-4C1A-9A89-E3180E619432}"/>
             </c:ext>
@@ -3706,27 +3714,27 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>61948.5</c:v>
+                  <c:v>24122</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>55193</c:v>
+                  <c:v>23989</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3604.5</c:v>
+                  <c:v>2284.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2266</c:v>
+                  <c:v>484</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2066.5</c:v>
+                  <c:v>477.5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2156.5</c:v>
+                  <c:v>570.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000004-6DCB-4C1A-9A89-E3180E619432}"/>
             </c:ext>
@@ -3742,11 +3750,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="817294175"/>
-        <c:axId val="823995663"/>
+        <c:axId val="246003192"/>
+        <c:axId val="246003584"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="817294175"/>
+        <c:axId val="246003192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3789,7 +3797,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="823995663"/>
+        <c:crossAx val="246003584"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3797,7 +3805,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="823995663"/>
+        <c:axId val="246003584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3848,7 +3856,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="817294175"/>
+        <c:crossAx val="246003192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3862,6 +3870,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3929,9 +3938,9 @@
 </file>
 
 <file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="da-DK"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -3968,6 +3977,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4072,25 +4082,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>290463</c:v>
+                  <c:v>99137.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>193442.5</c:v>
+                  <c:v>54961</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>148057</c:v>
+                  <c:v>36972.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>78329.5</c:v>
+                  <c:v>29082</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>61948.5</c:v>
+                  <c:v>24122</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-A320-4E6C-BF3F-9F2B7530DEC5}"/>
             </c:ext>
@@ -4165,25 +4175,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>268599</c:v>
+                  <c:v>81427</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>188385.5</c:v>
+                  <c:v>45044.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>130012</c:v>
+                  <c:v>32644</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>71834.5</c:v>
+                  <c:v>27281</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>55193</c:v>
+                  <c:v>23989</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-A320-4E6C-BF3F-9F2B7530DEC5}"/>
             </c:ext>
@@ -4258,25 +4268,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>19405.5</c:v>
+                  <c:v>20272</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>11636</c:v>
+                  <c:v>10361.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7101</c:v>
+                  <c:v>5550.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4595.5</c:v>
+                  <c:v>3162.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3604.5</c:v>
+                  <c:v>2284.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-A320-4E6C-BF3F-9F2B7530DEC5}"/>
             </c:ext>
@@ -4351,25 +4361,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>10493</c:v>
+                  <c:v>1751.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6072.5</c:v>
+                  <c:v>1047</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3469.5</c:v>
+                  <c:v>653.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2464.5</c:v>
+                  <c:v>463</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2266</c:v>
+                  <c:v>484</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000003-A320-4E6C-BF3F-9F2B7530DEC5}"/>
             </c:ext>
@@ -4444,25 +4454,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>10574</c:v>
+                  <c:v>1729.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6156.5</c:v>
+                  <c:v>1023</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3552</c:v>
+                  <c:v>632</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2441</c:v>
+                  <c:v>437</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2066.5</c:v>
+                  <c:v>477.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000004-A320-4E6C-BF3F-9F2B7530DEC5}"/>
             </c:ext>
@@ -4537,25 +4547,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>10577</c:v>
+                  <c:v>1791.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6277</c:v>
+                  <c:v>1097.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3635.5</c:v>
+                  <c:v>713.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2523.5</c:v>
+                  <c:v>553</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2156.5</c:v>
+                  <c:v>570.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000005-A320-4E6C-BF3F-9F2B7530DEC5}"/>
             </c:ext>
@@ -4571,11 +4581,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="922613247"/>
-        <c:axId val="816115151"/>
+        <c:axId val="246004368"/>
+        <c:axId val="246004760"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="922613247"/>
+        <c:axId val="246004368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4618,7 +4628,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="816115151"/>
+        <c:crossAx val="246004760"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4626,11 +4636,11 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="816115151"/>
+        <c:axId val="246004760"/>
         <c:scaling>
-          <c:logBase val="2"/>
           <c:orientation val="minMax"/>
-          <c:min val="2000"/>
+          <c:max val="100000"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -4679,7 +4689,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="922613247"/>
+        <c:crossAx val="246004368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4693,6 +4703,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4724,14 +4735,14 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:extLst>
+    <c:showDLblsOverMax val="0"/>
+    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
           <c16r3:dispNaAsBlank val="1"/>
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -8044,7 +8055,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{199DE40E-7BBF-4CA7-A4FF-08CEE051AD63}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{199DE40E-7BBF-4CA7-A4FF-08CEE051AD63}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8080,7 +8091,7 @@
         <xdr:cNvPr id="3" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3D4D81BA-2D4A-49AC-8613-4F3C140EAA10}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{3D4D81BA-2D4A-49AC-8613-4F3C140EAA10}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8116,7 +8127,7 @@
         <xdr:cNvPr id="4" name="Chart 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ED8FB22F-C6F2-4AF4-B0B6-01345E2E6DA0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{ED8FB22F-C6F2-4AF4-B0B6-01345E2E6DA0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8152,7 +8163,7 @@
         <xdr:cNvPr id="5" name="Chart 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DFDEB1F6-3BE7-4E5A-BC72-2D236B2083EB}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{DFDEB1F6-3BE7-4E5A-BC72-2D236B2083EB}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8188,7 +8199,7 @@
         <xdr:cNvPr id="6" name="Chart 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{23BA56C3-805A-4914-A127-4D913FE45377}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{23BA56C3-805A-4914-A127-4D913FE45377}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8226,7 +8237,7 @@
         <xdr:cNvPr id="7" name="Chart 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{46C10D9F-9929-4E0A-BC74-A794FD546A0C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{46C10D9F-9929-4E0A-BC74-A794FD546A0C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8511,7 +8522,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -9643,7 +9654,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D04218CA-24C1-4216-A555-E40A116FED1A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -10775,11 +10786,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF220BE2-5C84-44A4-A3B1-F5A09A2B5A64}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L53" sqref="L53"/>
+      <selection activeCell="M56" sqref="M56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10818,202 +10829,202 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>10595</v>
+        <v>1730</v>
       </c>
       <c r="C2">
-        <v>269352</v>
+        <v>81456</v>
       </c>
       <c r="E2">
-        <v>292085</v>
+        <v>99139</v>
       </c>
       <c r="G2">
-        <v>10499</v>
+        <v>1752</v>
       </c>
       <c r="I2">
-        <v>19462</v>
+        <v>20281</v>
       </c>
       <c r="K2">
-        <v>10578</v>
+        <v>1790</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>10574</v>
+        <v>1729</v>
       </c>
       <c r="C3">
-        <v>267732</v>
+        <v>81719</v>
       </c>
       <c r="E3">
-        <v>290648</v>
+        <v>99136</v>
       </c>
       <c r="G3">
-        <v>10491</v>
+        <v>1752</v>
       </c>
       <c r="I3">
-        <v>19405</v>
+        <v>20270</v>
       </c>
       <c r="K3">
-        <v>10575</v>
+        <v>1792</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>10571</v>
+        <v>1729</v>
       </c>
       <c r="C4">
-        <v>267943</v>
+        <v>81215</v>
       </c>
       <c r="E4">
-        <v>289805</v>
+        <v>98936</v>
       </c>
       <c r="G4">
-        <v>10498</v>
+        <v>1751</v>
       </c>
       <c r="I4">
-        <v>19404</v>
+        <v>20274</v>
       </c>
       <c r="K4">
-        <v>10574</v>
+        <v>1792</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>10574</v>
+        <v>1729</v>
       </c>
       <c r="C5">
-        <v>268490</v>
+        <v>81398</v>
       </c>
       <c r="E5">
-        <v>290592</v>
+        <v>99275</v>
       </c>
       <c r="G5">
-        <v>10506</v>
+        <v>1752</v>
       </c>
       <c r="I5">
-        <v>19413</v>
+        <v>20281</v>
       </c>
       <c r="K5">
-        <v>10577</v>
+        <v>1795</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>10572</v>
+        <v>1732</v>
       </c>
       <c r="C6">
-        <v>269095</v>
+        <v>81220</v>
       </c>
       <c r="E6">
-        <v>290756</v>
+        <v>99044</v>
       </c>
       <c r="G6">
-        <v>10492</v>
+        <v>1751</v>
       </c>
       <c r="I6">
-        <v>19405</v>
+        <v>20250</v>
       </c>
       <c r="K6">
-        <v>10577</v>
+        <v>1790</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>10605</v>
+        <v>1730</v>
       </c>
       <c r="C7">
-        <v>269549</v>
+        <v>81352</v>
       </c>
       <c r="E7">
-        <v>289443</v>
+        <v>98854</v>
       </c>
       <c r="G7">
-        <v>10505</v>
+        <v>1751</v>
       </c>
       <c r="I7">
-        <v>19408</v>
+        <v>20240</v>
       </c>
       <c r="K7">
-        <v>10580</v>
+        <v>1790</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>10574</v>
+        <v>1734</v>
       </c>
       <c r="C8">
-        <v>268309</v>
+        <v>81623</v>
       </c>
       <c r="E8">
-        <v>291622</v>
+        <v>99124</v>
       </c>
       <c r="G8">
-        <v>10491</v>
+        <v>1754</v>
       </c>
       <c r="I8">
-        <v>19403</v>
+        <v>20256</v>
       </c>
       <c r="K8">
-        <v>10579</v>
+        <v>1790</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>10574</v>
+        <v>1729</v>
       </c>
       <c r="C9">
-        <v>268708</v>
+        <v>81484</v>
       </c>
       <c r="E9">
-        <v>290334</v>
+        <v>99154</v>
       </c>
       <c r="G9">
-        <v>10493</v>
+        <v>1753</v>
       </c>
       <c r="I9">
-        <v>19407</v>
+        <v>20285</v>
       </c>
       <c r="K9">
-        <v>10580</v>
+        <v>1796</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>10573</v>
+        <v>1729</v>
       </c>
       <c r="C10">
-        <v>268004</v>
+        <v>81473</v>
       </c>
       <c r="E10">
-        <v>290313</v>
+        <v>99302</v>
       </c>
       <c r="G10">
-        <v>10493</v>
+        <v>1751</v>
       </c>
       <c r="I10">
-        <v>19406</v>
+        <v>20282</v>
       </c>
       <c r="K10">
-        <v>10576</v>
+        <v>1791</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>10588</v>
+        <v>1732</v>
       </c>
       <c r="C11">
-        <v>269721</v>
+        <v>81354</v>
       </c>
       <c r="E11">
-        <v>290186</v>
+        <v>99142</v>
       </c>
       <c r="G11">
-        <v>10492</v>
+        <v>1751</v>
       </c>
       <c r="I11">
-        <v>19401</v>
+        <v>20263</v>
       </c>
       <c r="K11">
-        <v>10575</v>
+        <v>1795</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -11038,202 +11049,202 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>6180</v>
+        <v>1021</v>
       </c>
       <c r="C14">
-        <v>189638</v>
+        <v>44990</v>
       </c>
       <c r="E14">
-        <v>191348</v>
+        <v>55221</v>
       </c>
       <c r="G14">
-        <v>6403</v>
+        <v>1047</v>
       </c>
       <c r="I14">
-        <v>11550</v>
+        <v>10347</v>
       </c>
       <c r="K14">
-        <v>6386</v>
+        <v>1098</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>6232</v>
+        <v>1026</v>
       </c>
       <c r="C15">
-        <v>172330</v>
+        <v>43319</v>
       </c>
       <c r="E15">
-        <v>220416</v>
+        <v>56348</v>
       </c>
       <c r="G15">
-        <v>5957</v>
+        <v>1049</v>
       </c>
       <c r="I15">
-        <v>11654</v>
+        <v>10310</v>
       </c>
       <c r="K15">
-        <v>6326</v>
+        <v>1107</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>6120</v>
+        <v>1022</v>
       </c>
       <c r="C16">
-        <v>175879</v>
+        <v>45117</v>
       </c>
       <c r="E16">
-        <v>188810</v>
+        <v>54064</v>
       </c>
       <c r="G16">
-        <v>6319</v>
+        <v>1047</v>
       </c>
       <c r="I16">
-        <v>11571</v>
+        <v>10490</v>
       </c>
       <c r="K16">
-        <v>6464</v>
+        <v>1093</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>5941</v>
+        <v>1023</v>
       </c>
       <c r="C17">
-        <v>219185</v>
+        <v>45033</v>
       </c>
       <c r="E17">
-        <v>192160</v>
+        <v>57585</v>
       </c>
       <c r="G17">
-        <v>6058</v>
+        <v>1036</v>
       </c>
       <c r="I17">
-        <v>11816</v>
+        <v>10355</v>
       </c>
       <c r="K17">
-        <v>6284</v>
+        <v>1115</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>6133</v>
+        <v>1022</v>
       </c>
       <c r="C18">
-        <v>200519</v>
+        <v>45365</v>
       </c>
       <c r="E18">
-        <v>190755</v>
+        <v>54811</v>
       </c>
       <c r="G18">
-        <v>6259</v>
+        <v>1044</v>
       </c>
       <c r="I18">
-        <v>11588</v>
+        <v>10399</v>
       </c>
       <c r="K18">
-        <v>6270</v>
+        <v>1093</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>6126</v>
+        <v>1024</v>
       </c>
       <c r="C19">
-        <v>174446</v>
+        <v>44945</v>
       </c>
       <c r="E19">
-        <v>194725</v>
+        <v>55933</v>
       </c>
       <c r="G19">
-        <v>5973</v>
+        <v>1056</v>
       </c>
       <c r="I19">
-        <v>11914</v>
+        <v>10369</v>
       </c>
       <c r="K19">
-        <v>6379</v>
+        <v>1097</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>6253</v>
+        <v>1023</v>
       </c>
       <c r="C20">
-        <v>216025</v>
+        <v>45155</v>
       </c>
       <c r="E20">
-        <v>209152</v>
+        <v>53647</v>
       </c>
       <c r="G20">
-        <v>6050</v>
+        <v>1056</v>
       </c>
       <c r="I20">
-        <v>11680</v>
+        <v>10346</v>
       </c>
       <c r="K20">
-        <v>6145</v>
+        <v>1095</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>6234</v>
+        <v>1026</v>
       </c>
       <c r="C21">
-        <v>187133</v>
+        <v>44323</v>
       </c>
       <c r="E21">
-        <v>191913</v>
+        <v>54673</v>
       </c>
       <c r="G21">
-        <v>6087</v>
+        <v>1043</v>
       </c>
       <c r="I21">
-        <v>11523</v>
+        <v>10527</v>
       </c>
       <c r="K21">
-        <v>6212</v>
+        <v>1093</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>6040</v>
+        <v>1023</v>
       </c>
       <c r="C22">
-        <v>182479</v>
+        <v>45188</v>
       </c>
       <c r="E22">
-        <v>196222</v>
+        <v>54855</v>
       </c>
       <c r="G22">
-        <v>6212</v>
+        <v>1052</v>
       </c>
       <c r="I22">
-        <v>12078</v>
+        <v>10348</v>
       </c>
       <c r="K22">
-        <v>6247</v>
+        <v>1104</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>6221</v>
+        <v>1023</v>
       </c>
       <c r="C23">
-        <v>190237</v>
+        <v>45056</v>
       </c>
       <c r="E23">
-        <v>195571</v>
+        <v>55067</v>
       </c>
       <c r="G23">
-        <v>6044</v>
+        <v>1034</v>
       </c>
       <c r="I23">
-        <v>11618</v>
+        <v>10368</v>
       </c>
       <c r="K23">
-        <v>6178</v>
+        <v>1103</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
@@ -11258,202 +11269,202 @@
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>3605</v>
+        <v>630</v>
       </c>
       <c r="C26">
-        <v>131095</v>
+        <v>31932</v>
       </c>
       <c r="E26">
-        <v>152242</v>
+        <v>36568</v>
       </c>
       <c r="G26">
-        <v>3400</v>
+        <v>668</v>
       </c>
       <c r="I26">
-        <v>7210</v>
+        <v>5622</v>
       </c>
       <c r="K26">
-        <v>3635</v>
+        <v>705</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>3466</v>
+        <v>633</v>
       </c>
       <c r="C27">
-        <v>130738</v>
+        <v>32724</v>
       </c>
       <c r="E27">
-        <v>154575</v>
+        <v>34010</v>
       </c>
       <c r="G27">
-        <v>3459</v>
+        <v>649</v>
       </c>
       <c r="I27">
-        <v>6671</v>
+        <v>5523</v>
       </c>
       <c r="K27">
-        <v>3877</v>
+        <v>722</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>3484</v>
+        <v>639</v>
       </c>
       <c r="C28">
-        <v>113585</v>
+        <v>31709</v>
       </c>
       <c r="E28">
-        <v>147381</v>
+        <v>39571</v>
       </c>
       <c r="G28">
-        <v>3534</v>
+        <v>654</v>
       </c>
       <c r="I28">
-        <v>7100</v>
+        <v>5559</v>
       </c>
       <c r="K28">
-        <v>3538</v>
+        <v>686</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>3582</v>
+        <v>674</v>
       </c>
       <c r="C29">
-        <v>128046</v>
+        <v>32901</v>
       </c>
       <c r="E29">
-        <v>137363</v>
+        <v>36108</v>
       </c>
       <c r="G29">
-        <v>3344</v>
+        <v>657</v>
       </c>
       <c r="I29">
-        <v>7521</v>
+        <v>5607</v>
       </c>
       <c r="K29">
-        <v>3673</v>
+        <v>730</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>3551</v>
+        <v>623</v>
       </c>
       <c r="C30">
-        <v>132934</v>
+        <v>34878</v>
       </c>
       <c r="E30">
-        <v>149459</v>
+        <v>34307</v>
       </c>
       <c r="G30">
-        <v>3446</v>
+        <v>648</v>
       </c>
       <c r="I30">
-        <v>7319</v>
+        <v>5537</v>
       </c>
       <c r="K30">
-        <v>3576</v>
+        <v>724</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>3600</v>
+        <v>631</v>
       </c>
       <c r="C31">
-        <v>131502</v>
+        <v>30048</v>
       </c>
       <c r="E31">
-        <v>148518</v>
+        <v>33997</v>
       </c>
       <c r="G31">
-        <v>3713</v>
+        <v>640</v>
       </c>
       <c r="I31">
-        <v>6060</v>
+        <v>5521</v>
       </c>
       <c r="K31">
-        <v>3696</v>
+        <v>713</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>3553</v>
+        <v>630</v>
       </c>
       <c r="C32">
-        <v>123246</v>
+        <v>32078</v>
       </c>
       <c r="E32">
-        <v>147596</v>
+        <v>40645</v>
       </c>
       <c r="G32">
-        <v>3326</v>
+        <v>653</v>
       </c>
       <c r="I32">
-        <v>6747</v>
+        <v>5405</v>
       </c>
       <c r="K32">
-        <v>3440</v>
+        <v>714</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>3384</v>
+        <v>629</v>
       </c>
       <c r="C33">
-        <v>132103</v>
+        <v>34659</v>
       </c>
       <c r="E33">
-        <v>144939</v>
+        <v>37551</v>
       </c>
       <c r="G33">
-        <v>3480</v>
+        <v>647</v>
       </c>
       <c r="I33">
-        <v>7298</v>
+        <v>5542</v>
       </c>
       <c r="K33">
-        <v>3636</v>
+        <v>710</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>3528</v>
+        <v>634</v>
       </c>
       <c r="C34">
-        <v>114714</v>
+        <v>32564</v>
       </c>
       <c r="E34">
-        <v>143547</v>
+        <v>37377</v>
       </c>
       <c r="G34">
-        <v>3881</v>
+        <v>693</v>
       </c>
       <c r="I34">
-        <v>7102</v>
+        <v>5565</v>
       </c>
       <c r="K34">
-        <v>3609</v>
+        <v>745</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>3668</v>
+        <v>675</v>
       </c>
       <c r="C35">
-        <v>129286</v>
+        <v>32916</v>
       </c>
       <c r="E35">
-        <v>149978</v>
+        <v>38815</v>
       </c>
       <c r="G35">
-        <v>3586</v>
+        <v>662</v>
       </c>
       <c r="I35">
-        <v>6848</v>
+        <v>5673</v>
       </c>
       <c r="K35">
-        <v>3751</v>
+        <v>703</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
@@ -11478,202 +11489,202 @@
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38">
-        <v>2189</v>
+        <v>435</v>
       </c>
       <c r="C38">
-        <v>73721</v>
+        <v>26494</v>
       </c>
       <c r="E38">
-        <v>75434</v>
+        <v>28410</v>
       </c>
       <c r="G38">
-        <v>2499</v>
+        <v>560</v>
       </c>
       <c r="I38">
-        <v>4726</v>
+        <v>3289</v>
       </c>
       <c r="K38">
-        <v>2325</v>
+        <v>504</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39">
-        <v>2799</v>
+        <v>425</v>
       </c>
       <c r="C39">
-        <v>66663</v>
+        <v>28119</v>
       </c>
       <c r="E39">
-        <v>80343</v>
+        <v>26292</v>
       </c>
       <c r="G39">
-        <v>2129</v>
+        <v>452</v>
       </c>
       <c r="I39">
-        <v>4788</v>
+        <v>3119</v>
       </c>
       <c r="K39">
-        <v>2383</v>
+        <v>647</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40">
-        <v>2146</v>
+        <v>415</v>
       </c>
       <c r="C40">
-        <v>71951</v>
+        <v>28097</v>
       </c>
       <c r="E40">
-        <v>71385</v>
+        <v>28958</v>
       </c>
       <c r="G40">
-        <v>2628</v>
+        <v>454</v>
       </c>
       <c r="I40">
-        <v>4699</v>
+        <v>2945</v>
       </c>
       <c r="K40">
-        <v>2634</v>
+        <v>535</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41">
-        <v>2563</v>
+        <v>490</v>
       </c>
       <c r="C41">
-        <v>73996</v>
+        <v>26861</v>
       </c>
       <c r="E41">
-        <v>79529</v>
+        <v>29737</v>
       </c>
       <c r="G41">
-        <v>2269</v>
+        <v>477</v>
       </c>
       <c r="I41">
-        <v>4420</v>
+        <v>3473</v>
       </c>
       <c r="K41">
-        <v>2406</v>
+        <v>567</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42">
-        <v>2718</v>
+        <v>439</v>
       </c>
       <c r="C42">
-        <v>71718</v>
+        <v>25249</v>
       </c>
       <c r="E42">
-        <v>78036</v>
+        <v>28681</v>
       </c>
       <c r="G42">
-        <v>2646</v>
+        <v>455</v>
       </c>
       <c r="I42">
-        <v>4318</v>
+        <v>3307</v>
       </c>
       <c r="K42">
-        <v>2413</v>
+        <v>491</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43">
-        <v>2463</v>
+        <v>469</v>
       </c>
       <c r="C43">
-        <v>74680</v>
+        <v>27489</v>
       </c>
       <c r="E43">
-        <v>85540</v>
+        <v>29833</v>
       </c>
       <c r="G43">
-        <v>2250</v>
+        <v>451</v>
       </c>
       <c r="I43">
-        <v>4492</v>
+        <v>3045</v>
       </c>
       <c r="K43">
-        <v>2657</v>
+        <v>571</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44">
-        <v>2781</v>
+        <v>431</v>
       </c>
       <c r="C44">
-        <v>71429</v>
+        <v>27073</v>
       </c>
       <c r="E44">
-        <v>74463</v>
+        <v>29206</v>
       </c>
       <c r="G44">
-        <v>2518</v>
+        <v>471</v>
       </c>
       <c r="I44">
-        <v>4158</v>
+        <v>3358</v>
       </c>
       <c r="K44">
-        <v>2805</v>
+        <v>495</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45">
-        <v>2419</v>
+        <v>496</v>
       </c>
       <c r="C45">
-        <v>71240</v>
+        <v>29000</v>
       </c>
       <c r="E45">
-        <v>72655</v>
+        <v>29890</v>
       </c>
       <c r="G45">
-        <v>2430</v>
+        <v>490</v>
       </c>
       <c r="I45">
-        <v>5091</v>
+        <v>3123</v>
       </c>
       <c r="K45">
-        <v>2406</v>
+        <v>702</v>
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46">
-        <v>2340</v>
+        <v>431</v>
       </c>
       <c r="C46">
-        <v>77192</v>
+        <v>25764</v>
       </c>
       <c r="E46">
-        <v>83051</v>
+        <v>27276</v>
       </c>
       <c r="G46">
-        <v>1996</v>
+        <v>448</v>
       </c>
       <c r="I46">
-        <v>5243</v>
+        <v>3099</v>
       </c>
       <c r="K46">
-        <v>2656</v>
+        <v>539</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47">
-        <v>2383</v>
+        <v>527</v>
       </c>
       <c r="C47">
-        <v>64226</v>
+        <v>29089</v>
       </c>
       <c r="E47">
-        <v>78623</v>
+        <v>29758</v>
       </c>
       <c r="G47">
-        <v>2612</v>
+        <v>557</v>
       </c>
       <c r="I47">
-        <v>4409</v>
+        <v>3202</v>
       </c>
       <c r="K47">
-        <v>2746</v>
+        <v>648</v>
       </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.25">
@@ -11698,202 +11709,202 @@
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50">
-        <v>6726</v>
+        <v>458</v>
       </c>
       <c r="C50">
-        <v>60975</v>
+        <v>25426</v>
       </c>
       <c r="E50">
-        <v>59503</v>
+        <v>28889</v>
       </c>
       <c r="G50">
-        <v>2162</v>
+        <v>525</v>
       </c>
       <c r="I50">
-        <v>3582</v>
+        <v>2263</v>
       </c>
       <c r="K50">
-        <v>2144</v>
+        <v>534</v>
       </c>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51">
-        <v>2282</v>
+        <v>485</v>
       </c>
       <c r="C51">
-        <v>54393</v>
+        <v>25822</v>
       </c>
       <c r="E51">
-        <v>62091</v>
+        <v>24251</v>
       </c>
       <c r="G51">
-        <v>2516</v>
+        <v>487</v>
       </c>
       <c r="I51">
-        <v>3567</v>
+        <v>2379</v>
       </c>
       <c r="K51">
-        <v>2146</v>
+        <v>680</v>
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52">
-        <v>2077</v>
+        <v>481</v>
       </c>
       <c r="C52">
-        <v>58435</v>
+        <v>22335</v>
       </c>
       <c r="E52">
-        <v>62508</v>
+        <v>23376</v>
       </c>
       <c r="G52">
-        <v>2106</v>
+        <v>483</v>
       </c>
       <c r="I52">
-        <v>7559</v>
+        <v>2272</v>
       </c>
       <c r="K52">
-        <v>2623</v>
+        <v>553</v>
       </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53">
-        <v>1985</v>
+        <v>474</v>
       </c>
       <c r="C53">
-        <v>55419</v>
+        <v>23857</v>
       </c>
       <c r="E53">
-        <v>64752</v>
+        <v>22459</v>
       </c>
       <c r="G53">
-        <v>2316</v>
+        <v>478</v>
       </c>
       <c r="I53">
-        <v>5037</v>
+        <v>2605</v>
       </c>
       <c r="K53">
-        <v>2167</v>
+        <v>647</v>
       </c>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54">
-        <v>1997</v>
+        <v>451</v>
       </c>
       <c r="C54">
-        <v>54108</v>
+        <v>24279</v>
       </c>
       <c r="E54">
-        <v>60897</v>
+        <v>22816</v>
       </c>
       <c r="G54">
-        <v>2029</v>
+        <v>485</v>
       </c>
       <c r="I54">
-        <v>3514</v>
+        <v>2910</v>
       </c>
       <c r="K54">
-        <v>2131</v>
+        <v>555</v>
       </c>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55">
-        <v>3056</v>
+        <v>473</v>
       </c>
       <c r="C55">
-        <v>52803</v>
+        <v>26419</v>
       </c>
       <c r="E55">
-        <v>63126</v>
+        <v>24087</v>
       </c>
       <c r="G55">
-        <v>2057</v>
+        <v>481</v>
       </c>
       <c r="I55">
-        <v>3559</v>
+        <v>2283</v>
       </c>
       <c r="K55">
-        <v>2311</v>
+        <v>553</v>
       </c>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56">
-        <v>2020</v>
+        <v>471</v>
       </c>
       <c r="C56">
-        <v>54500</v>
+        <v>23658</v>
       </c>
       <c r="E56">
-        <v>59916</v>
+        <v>22799</v>
       </c>
       <c r="G56">
-        <v>3841</v>
+        <v>497</v>
       </c>
       <c r="I56">
-        <v>3627</v>
+        <v>2277</v>
       </c>
       <c r="K56">
-        <v>2255</v>
+        <v>647</v>
       </c>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57">
-        <v>2056</v>
+        <v>493</v>
       </c>
       <c r="C57">
-        <v>54967</v>
+        <v>24121</v>
       </c>
       <c r="E57">
-        <v>61806</v>
+        <v>24157</v>
       </c>
       <c r="G57">
-        <v>2877</v>
+        <v>483</v>
       </c>
       <c r="I57">
-        <v>3541</v>
+        <v>4942</v>
       </c>
       <c r="K57">
-        <v>2145</v>
+        <v>586</v>
       </c>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58">
-        <v>2055</v>
+        <v>863</v>
       </c>
       <c r="C58">
-        <v>58238</v>
+        <v>22240</v>
       </c>
       <c r="E58">
-        <v>64360</v>
+        <v>24356</v>
       </c>
       <c r="G58">
-        <v>2216</v>
+        <v>478</v>
       </c>
       <c r="I58">
-        <v>4181</v>
+        <v>2286</v>
       </c>
       <c r="K58">
-        <v>2214</v>
+        <v>552</v>
       </c>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59">
-        <v>2225</v>
+        <v>644</v>
       </c>
       <c r="C59">
-        <v>57433</v>
+        <v>23198</v>
       </c>
       <c r="E59">
-        <v>59233</v>
+        <v>24751</v>
       </c>
       <c r="G59">
-        <v>2668</v>
+        <v>486</v>
       </c>
       <c r="I59">
-        <v>4025</v>
+        <v>2275</v>
       </c>
       <c r="K59">
-        <v>2113</v>
+        <v>761</v>
       </c>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.25">
@@ -11907,11 +11918,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B6641D4-9D9F-437B-BDC3-57FD62A69C2D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="X28" sqref="X28"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12276,23 +12287,23 @@
       </c>
       <c r="B16">
         <f>MEDIAN(Google!E$2:E$11)</f>
-        <v>290463</v>
+        <v>99137.5</v>
       </c>
       <c r="C16">
         <f>MEDIAN(Google!E$14:E$23)</f>
-        <v>193442.5</v>
+        <v>54961</v>
       </c>
       <c r="D16">
         <f>MEDIAN(Google!E$26:E$35)</f>
-        <v>148057</v>
+        <v>36972.5</v>
       </c>
       <c r="E16">
         <f>MEDIAN(Google!E$38:E$47)</f>
-        <v>78329.5</v>
+        <v>29082</v>
       </c>
       <c r="F16">
         <f>MEDIAN(Google!E$50:E$59)</f>
-        <v>61948.5</v>
+        <v>24122</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -12301,23 +12312,23 @@
       </c>
       <c r="B17">
         <f>MEDIAN(Google!C$2:C$11)</f>
-        <v>268599</v>
+        <v>81427</v>
       </c>
       <c r="C17">
         <f>MEDIAN(Google!C$14:C$23)</f>
-        <v>188385.5</v>
+        <v>45044.5</v>
       </c>
       <c r="D17">
         <f>MEDIAN(Google!C$26:C$35)</f>
-        <v>130012</v>
+        <v>32644</v>
       </c>
       <c r="E17">
         <f>MEDIAN(Google!C$38:C$47)</f>
-        <v>71834.5</v>
+        <v>27281</v>
       </c>
       <c r="F17">
         <f>MEDIAN(Google!C$50:C$59)</f>
-        <v>55193</v>
+        <v>23989</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -12326,23 +12337,23 @@
       </c>
       <c r="B18">
         <f>MEDIAN(Google!I$2:I$11)</f>
-        <v>19405.5</v>
+        <v>20272</v>
       </c>
       <c r="C18">
         <f>MEDIAN(Google!I$14:I$23)</f>
-        <v>11636</v>
+        <v>10361.5</v>
       </c>
       <c r="D18">
         <f>MEDIAN(Google!I$26:I$35)</f>
-        <v>7101</v>
+        <v>5550.5</v>
       </c>
       <c r="E18">
         <f>MEDIAN(Google!I$38:I$47)</f>
-        <v>4595.5</v>
+        <v>3162.5</v>
       </c>
       <c r="F18">
         <f>MEDIAN(Google!I$50:I$59)</f>
-        <v>3604.5</v>
+        <v>2284.5</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -12351,23 +12362,23 @@
       </c>
       <c r="B19">
         <f>MEDIAN(Google!G$2:G$11)</f>
-        <v>10493</v>
+        <v>1751.5</v>
       </c>
       <c r="C19">
         <f>MEDIAN(Google!G$14:G$23)</f>
-        <v>6072.5</v>
+        <v>1047</v>
       </c>
       <c r="D19">
         <f>MEDIAN(Google!G$26:G$35)</f>
-        <v>3469.5</v>
+        <v>653.5</v>
       </c>
       <c r="E19">
         <f>MEDIAN(Google!G$38:G$47)</f>
-        <v>2464.5</v>
+        <v>463</v>
       </c>
       <c r="F19">
         <f>MEDIAN(Google!G$50:G$59)</f>
-        <v>2266</v>
+        <v>484</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -12376,23 +12387,23 @@
       </c>
       <c r="B20">
         <f>MEDIAN(Google!A$2:A$11)</f>
-        <v>10574</v>
+        <v>1729.5</v>
       </c>
       <c r="C20">
         <f>MEDIAN(Google!A$14:A$23)</f>
-        <v>6156.5</v>
+        <v>1023</v>
       </c>
       <c r="D20">
         <f>MEDIAN(Google!A$26:A$35)</f>
-        <v>3552</v>
+        <v>632</v>
       </c>
       <c r="E20">
         <f>MEDIAN(Google!A$38:A$47)</f>
-        <v>2441</v>
+        <v>437</v>
       </c>
       <c r="F20">
         <f>MEDIAN(Google!A$50:A$59)</f>
-        <v>2066.5</v>
+        <v>477.5</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -12401,23 +12412,23 @@
       </c>
       <c r="B21">
         <f>MEDIAN(Google!K$2:K$11)</f>
-        <v>10577</v>
+        <v>1791.5</v>
       </c>
       <c r="C21">
         <f>MEDIAN(Google!K$14:K$23)</f>
-        <v>6277</v>
+        <v>1097.5</v>
       </c>
       <c r="D21">
         <f>MEDIAN(Google!K$26:K$35)</f>
-        <v>3635.5</v>
+        <v>713.5</v>
       </c>
       <c r="E21">
         <f>MEDIAN(Google!K$38:K$47)</f>
-        <v>2523.5</v>
+        <v>553</v>
       </c>
       <c r="F21">
         <f>MEDIAN(Google!K$50:K$59)</f>
-        <v>2156.5</v>
+        <v>570.5</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>